<commit_message>
Add eu2 - p&p
Using Binet's formula for Fibonacci numbers.
Sum of geometric series.
</commit_message>
<xml_diff>
--- a/00 index.xlsx
+++ b/00 index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="398">
   <si>
     <t>Number</t>
   </si>
@@ -1205,6 +1205,9 @@
   </si>
   <si>
     <t>~about 1 minute</t>
+  </si>
+  <si>
+    <t>Pen &amp; Paper</t>
   </si>
 </sst>
 </file>
@@ -1608,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H244" sqref="H244"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,11 +1620,12 @@
     <col min="1" max="1" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="99.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="115.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="22" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1649,6 +1653,9 @@
       <c r="H1" s="2" t="s">
         <v>233</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -1667,7 +1674,9 @@
       <c r="H2" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1687,7 +1696,9 @@
       <c r="H3" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add eu28 - p&p
Using formula for sum of consecutive squares, and consecutive integers.
</commit_message>
<xml_diff>
--- a/00 index.xlsx
+++ b/00 index.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="410">
   <si>
     <t>Number</t>
   </si>
@@ -1238,6 +1238,12 @@
   </si>
   <si>
     <t>~about 30 secs</t>
+  </si>
+  <si>
+    <t>272, 421</t>
+  </si>
+  <si>
+    <t>271, 421</t>
   </si>
 </sst>
 </file>
@@ -1639,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J459"/>
+  <dimension ref="A1:J465"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C196" sqref="C196"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E229" sqref="E229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5145,91 +5151,79 @@
       <c r="I211" s="1"/>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>233</v>
+      </c>
+      <c r="E212" s="3">
+        <v>354</v>
+      </c>
       <c r="I212" s="1"/>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A213" s="1">
-        <v>243</v>
-      </c>
       <c r="I213" s="1"/>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I214" s="1"/>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>243</v>
+      </c>
       <c r="I215" s="1"/>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A216" s="1">
+      <c r="I216" s="1"/>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I217" s="1"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
         <v>248</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="B218" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D216" s="3" t="s">
+      <c r="D218" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="E216" s="3">
+      <c r="E218" s="3">
         <v>72</v>
       </c>
-      <c r="F216" s="11">
+      <c r="F218" s="11">
         <v>23507044290</v>
       </c>
-      <c r="G216" s="5">
+      <c r="G218" s="5">
         <v>41798</v>
       </c>
-      <c r="H216" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="I216" s="1"/>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G217" s="5"/>
-      <c r="I217" s="1"/>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G218" s="5"/>
+      <c r="H218" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I218" s="1"/>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A219" s="1">
-        <v>265</v>
-      </c>
-      <c r="B219" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D219" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F219" s="11">
-        <v>209110240768</v>
-      </c>
-      <c r="G219" s="5">
-        <v>42190</v>
-      </c>
-      <c r="H219" s="1" t="s">
-        <v>320</v>
-      </c>
+      <c r="G219" s="5"/>
       <c r="I219" s="1"/>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G220" s="5"/>
       <c r="I220" s="1"/>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="F221" s="16" t="s">
-        <v>388</v>
+        <v>379</v>
+      </c>
+      <c r="F221" s="11">
+        <v>209110240768</v>
       </c>
       <c r="G221" s="5">
-        <v>42200</v>
+        <v>42190</v>
       </c>
       <c r="H221" s="1" t="s">
         <v>320</v>
@@ -5240,30 +5234,30 @@
       <c r="I222" s="1"/>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>267</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F223" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="G223" s="5">
+        <v>42200</v>
+      </c>
+      <c r="H223" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I223" s="1"/>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I224" s="1"/>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A225" s="1">
-        <v>271</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="D225" s="3" t="s">
-        <v>369</v>
-      </c>
-      <c r="F225" s="16" t="s">
-        <v>368</v>
-      </c>
-      <c r="G225" s="5">
-        <v>41897</v>
-      </c>
-      <c r="H225" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="I225" s="1"/>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
@@ -5271,35 +5265,42 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>301</v>
+        <v>271</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>49</v>
+        <v>265</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>14</v>
+        <v>369</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="F227" s="16" t="s">
+        <v>368</v>
       </c>
       <c r="G227" s="5">
-        <v>41746</v>
+        <v>41897</v>
+      </c>
+      <c r="H227" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="I227" s="1"/>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>272</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="F228" s="16"/>
+      <c r="G228" s="5"/>
       <c r="I228" s="1"/>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A229" s="1">
-        <v>303</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D229" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G229" s="5">
-        <v>41784</v>
-      </c>
+      <c r="F229" s="16"/>
+      <c r="G229" s="5"/>
       <c r="I229" s="1"/>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
@@ -5307,10 +5308,16 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>305</v>
-      </c>
-      <c r="E231" s="3">
-        <v>40</v>
+        <v>301</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G231" s="5">
+        <v>41746</v>
       </c>
       <c r="I231" s="1"/>
     </row>
@@ -5318,60 +5325,54 @@
       <c r="I232" s="1"/>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>303</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G233" s="5">
+        <v>41784</v>
+      </c>
       <c r="I233" s="1"/>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A234" s="1">
+      <c r="I234" s="1"/>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>305</v>
+      </c>
+      <c r="E235" s="3">
+        <v>40</v>
+      </c>
+      <c r="I235" s="1"/>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I236" s="1"/>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I237" s="1"/>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
         <v>308</v>
       </c>
-      <c r="B234" s="1" t="s">
+      <c r="B238" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="F234" s="11">
+      <c r="F238" s="11">
         <v>1539669807660920</v>
       </c>
-      <c r="G234" s="5">
+      <c r="G238" s="5">
         <v>41941</v>
       </c>
-      <c r="H234" s="1" t="s">
+      <c r="H238" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="I234" s="1"/>
-    </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G235" s="5"/>
-      <c r="I235" s="1"/>
-    </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G236" s="5"/>
-      <c r="I236" s="1"/>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A237" s="1">
-        <v>315</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D237" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="E237" s="3">
-        <v>159</v>
-      </c>
-      <c r="F237" s="11">
-        <v>13625242</v>
-      </c>
-      <c r="G237" s="5">
-        <v>42161</v>
-      </c>
-      <c r="H237" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="I237" s="1"/>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G238" s="5"/>
       <c r="I238" s="1"/>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.25">
@@ -5379,26 +5380,31 @@
       <c r="I239" s="1"/>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A240" s="1">
-        <v>323</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="F240" s="16" t="s">
-        <v>340</v>
-      </c>
-      <c r="G240" s="5">
-        <v>42069</v>
-      </c>
-      <c r="H240" s="1" t="s">
-        <v>320</v>
-      </c>
+      <c r="G240" s="5"/>
       <c r="I240" s="1"/>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F241" s="16"/>
-      <c r="G241" s="5"/>
+      <c r="A241" s="1">
+        <v>315</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E241" s="3">
+        <v>159</v>
+      </c>
+      <c r="F241" s="11">
+        <v>13625242</v>
+      </c>
+      <c r="G241" s="5">
+        <v>42161</v>
+      </c>
+      <c r="H241" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I241" s="1"/>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.25">
@@ -5406,20 +5412,18 @@
       <c r="I242" s="1"/>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G243" s="5"/>
       <c r="I243" s="1"/>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="D244" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="F244" s="11" t="s">
-        <v>337</v>
+        <v>339</v>
+      </c>
+      <c r="F244" s="16" t="s">
+        <v>340</v>
       </c>
       <c r="G244" s="5">
         <v>42069</v>
@@ -5430,188 +5434,181 @@
       <c r="I244" s="1"/>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F245" s="16"/>
+      <c r="G245" s="5"/>
       <c r="I245" s="1"/>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G246" s="5"/>
       <c r="I246" s="1"/>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A247" s="1">
-        <v>336</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="D247" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="F247" s="11" t="s">
-        <v>391</v>
-      </c>
-      <c r="G247" s="5">
-        <v>42201</v>
-      </c>
-      <c r="H247" s="1" t="s">
-        <v>396</v>
-      </c>
       <c r="I247" s="1"/>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>329</v>
+      </c>
+      <c r="B248" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="D248" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="F248" s="11" t="s">
+        <v>337</v>
+      </c>
+      <c r="G248" s="5">
+        <v>42069</v>
+      </c>
+      <c r="H248" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I248" s="1"/>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I249" s="1"/>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A250" s="1">
-        <v>345</v>
-      </c>
-      <c r="B250" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D250" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="F250" s="11">
-        <v>13938</v>
-      </c>
-      <c r="G250" s="5">
-        <v>42010</v>
-      </c>
-      <c r="H250" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="I250" s="1"/>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
+        <v>336</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D251" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F251" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="G251" s="5">
+        <v>42201</v>
+      </c>
+      <c r="H251" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="I251" s="1"/>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I252" s="1"/>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I253" s="1"/>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>345</v>
+      </c>
+      <c r="B254" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D254" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="F254" s="11">
+        <v>13938</v>
+      </c>
+      <c r="G254" s="5">
+        <v>42010</v>
+      </c>
+      <c r="H254" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="I254" s="1"/>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
         <v>346</v>
       </c>
-      <c r="B251" s="1" t="s">
+      <c r="B255" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="F251" s="11">
+      <c r="F255" s="11">
         <v>3.3610879768925901E+17</v>
       </c>
-      <c r="G251" s="5">
+      <c r="G255" s="5">
         <v>42200</v>
       </c>
-      <c r="H251" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="I251" s="1"/>
-    </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A252" s="1">
-        <v>347</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="D252" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="F252" s="11">
-        <v>11109800204052</v>
-      </c>
-      <c r="G252" s="5">
-        <v>42200</v>
-      </c>
-      <c r="H252" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="I252" s="1"/>
-    </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G253" s="5"/>
-      <c r="I253" s="1"/>
-    </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G254" s="5"/>
-      <c r="I254" s="1"/>
-    </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H255" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I255" s="1"/>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
+        <v>347</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D256" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="F256" s="11">
+        <v>11109800204052</v>
+      </c>
+      <c r="G256" s="5">
+        <v>42200</v>
+      </c>
+      <c r="H256" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="I256" s="1"/>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G257" s="5"/>
+      <c r="I257" s="1"/>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G258" s="5"/>
+      <c r="I258" s="1"/>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>354</v>
+      </c>
+      <c r="E259" s="3">
+        <v>233</v>
+      </c>
+      <c r="G259" s="5"/>
+      <c r="I259" s="1"/>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G260" s="5"/>
+      <c r="I260" s="1"/>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I261" s="1"/>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
         <v>357</v>
       </c>
-      <c r="B256" s="1" t="s">
+      <c r="B262" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="D256" s="3" t="s">
+      <c r="D262" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="F256" s="11">
+      <c r="F262" s="11">
         <v>1739023853137</v>
       </c>
-      <c r="G256" s="3" t="s">
+      <c r="G262" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="H256" s="1" t="s">
+      <c r="H262" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="I256" s="1"/>
-    </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I257" s="1"/>
-    </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I258" s="1"/>
-    </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I259" s="1"/>
-    </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I260" s="1"/>
-    </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A261" s="1">
-        <v>381</v>
-      </c>
-      <c r="B261" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="D261" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F261" s="11">
-        <v>139602943319822</v>
-      </c>
-      <c r="G261" s="5">
-        <v>42100</v>
-      </c>
-      <c r="H261" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="I261" s="1"/>
-    </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I262" s="1"/>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I263" s="1"/>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A264" s="1">
-        <v>387</v>
-      </c>
-      <c r="B264" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D264" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="F264" s="11">
-        <v>696067597313468</v>
-      </c>
-      <c r="G264" s="5">
-        <v>42173</v>
-      </c>
-      <c r="H264" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="I264" s="1"/>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.25">
@@ -5622,25 +5619,22 @@
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
-        <v>429</v>
+        <v>381</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>406</v>
+        <v>350</v>
       </c>
       <c r="D267" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="E267" s="3">
-        <v>203</v>
+        <v>351</v>
       </c>
       <c r="F267" s="11">
-        <v>98792821</v>
+        <v>139602943319822</v>
       </c>
       <c r="G267" s="5">
-        <v>42209</v>
+        <v>42100</v>
       </c>
       <c r="H267" s="1" t="s">
-        <v>407</v>
+        <v>352</v>
       </c>
       <c r="I267" s="1"/>
     </row>
@@ -5651,57 +5645,57 @@
       <c r="I269" s="1"/>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>387</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D270" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F270" s="11">
+        <v>696067597313468</v>
+      </c>
+      <c r="G270" s="5">
+        <v>42173</v>
+      </c>
+      <c r="H270" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I270" s="1"/>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A271" s="1">
-        <v>435</v>
-      </c>
-      <c r="B271" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="D271" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="E271" s="3">
-        <v>137</v>
-      </c>
-      <c r="F271" s="11">
-        <v>252541322550</v>
-      </c>
-      <c r="G271" s="5">
-        <v>42178</v>
-      </c>
-      <c r="H271" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="I271" s="1"/>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I272" s="1"/>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
+        <v>429</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D273" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="E273" s="3">
+        <v>203</v>
+      </c>
+      <c r="F273" s="11">
+        <v>98792821</v>
+      </c>
+      <c r="G273" s="5">
+        <v>42209</v>
+      </c>
+      <c r="H273" s="1" t="s">
+        <v>407</v>
+      </c>
       <c r="I273" s="1"/>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A274" s="1">
-        <v>493</v>
-      </c>
-      <c r="B274" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D274" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="F274" s="16" t="s">
-        <v>341</v>
-      </c>
-      <c r="G274" s="5">
-        <v>42069</v>
-      </c>
-      <c r="H274" s="1" t="s">
-        <v>320</v>
-      </c>
       <c r="I274" s="1"/>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.25">
@@ -5711,6 +5705,27 @@
       <c r="I276" s="1"/>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>435</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D277" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="E277" s="3">
+        <v>137</v>
+      </c>
+      <c r="F277" s="11">
+        <v>252541322550</v>
+      </c>
+      <c r="G277" s="5">
+        <v>42178</v>
+      </c>
+      <c r="H277" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I277" s="1"/>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.25">
@@ -5721,16 +5736,16 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D280" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="F280" s="11">
-        <v>35407281</v>
+        <v>301</v>
+      </c>
+      <c r="F280" s="16" t="s">
+        <v>341</v>
       </c>
       <c r="G280" s="5">
         <v>42069</v>
@@ -5750,30 +5765,30 @@
       <c r="I283" s="1"/>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A284" s="1">
-        <v>504</v>
-      </c>
-      <c r="B284" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="D284" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="F284" s="11">
-        <v>694687</v>
-      </c>
-      <c r="G284" s="5">
-        <v>42209</v>
-      </c>
-      <c r="H284" s="1" t="s">
-        <v>404</v>
-      </c>
       <c r="I284" s="1"/>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I285" s="1"/>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A286" s="1">
+        <v>500</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="F286" s="11">
+        <v>35407281</v>
+      </c>
+      <c r="G286" s="5">
+        <v>42069</v>
+      </c>
+      <c r="H286" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I286" s="1"/>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.25">
@@ -5787,25 +5802,22 @@
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>370</v>
+        <v>402</v>
       </c>
       <c r="D290" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="E290" s="3" t="s">
-        <v>319</v>
+        <v>403</v>
       </c>
       <c r="F290" s="11">
-        <v>939087315</v>
+        <v>694687</v>
       </c>
       <c r="G290" s="5">
-        <v>42171</v>
+        <v>42209</v>
       </c>
       <c r="H290" s="1" t="s">
-        <v>372</v>
+        <v>404</v>
       </c>
       <c r="I290" s="1"/>
     </row>
@@ -5825,6 +5837,27 @@
       <c r="I295" s="1"/>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A296" s="1">
+        <v>516</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="D296" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E296" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F296" s="11">
+        <v>939087315</v>
+      </c>
+      <c r="G296" s="5">
+        <v>42171</v>
+      </c>
+      <c r="H296" s="1" t="s">
+        <v>372</v>
+      </c>
       <c r="I296" s="1"/>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.25">
@@ -6315,6 +6348,24 @@
     </row>
     <row r="459" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I459" s="1"/>
+    </row>
+    <row r="460" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I460" s="1"/>
+    </row>
+    <row r="461" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I461" s="1"/>
+    </row>
+    <row r="462" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I462" s="1"/>
+    </row>
+    <row r="463" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I463" s="1"/>
+    </row>
+    <row r="464" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I464" s="1"/>
+    </row>
+    <row r="465" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I465" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add eu601 + p&p
Key observation and simple counting.
</commit_message>
<xml_diff>
--- a/00 index.xlsx
+++ b/00 index.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="0" windowWidth="2130" windowHeight="0"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4652" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4654" uniqueCount="441">
   <si>
     <t>Number</t>
   </si>
@@ -1334,12 +1334,15 @@
   </si>
   <si>
     <t>prime_sieve; is_probable_prime; check200; check_prime_proof</t>
+  </si>
+  <si>
+    <t>Divisibility streaks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
@@ -1524,6 +1527,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1559,6 +1579,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1737,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F193" sqref="F193"/>
+    <sheetView tabSelected="1" topLeftCell="A281" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A326" sqref="A326:H326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41081,6 +41118,21 @@
       <c r="I325" s="1"/>
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A326" s="1">
+        <v>601</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="F326" s="11">
+        <v>1617243</v>
+      </c>
+      <c r="G326" s="5">
+        <v>42855</v>
+      </c>
+      <c r="H326" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I326" s="1"/>
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add eu613 + p&p
Using scipy integrate.
</commit_message>
<xml_diff>
--- a/00 index.xlsx
+++ b/00 index.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="0" windowWidth="2130" windowHeight="0"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="445">
   <si>
     <t>Number</t>
   </si>
@@ -1343,15 +1343,22 @@
   </si>
   <si>
     <t>fsolve (scipy)</t>
+  </si>
+  <si>
+    <t>Pythagorean Ant</t>
+  </si>
+  <si>
+    <t>integrate (scipy)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1390,7 +1397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1438,6 +1445,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1781,7 +1791,7 @@
   <dimension ref="A1:J485"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A281" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A291" sqref="A291:XFD291"/>
+      <selection activeCell="A338" sqref="A338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6392,52 +6402,70 @@
     <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I336" s="1"/>
     </row>
-    <row r="337" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>613</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D337" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="F337" s="17">
+        <v>0.39167215039999997</v>
+      </c>
+      <c r="G337" s="5">
+        <v>43117</v>
+      </c>
+      <c r="H337" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="I337" s="1"/>
     </row>
-    <row r="338" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I338" s="1"/>
     </row>
-    <row r="339" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I339" s="1"/>
     </row>
-    <row r="340" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I340" s="1"/>
     </row>
-    <row r="341" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I341" s="1"/>
     </row>
-    <row r="342" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I342" s="1"/>
     </row>
-    <row r="343" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I343" s="1"/>
     </row>
-    <row r="344" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I344" s="1"/>
     </row>
-    <row r="345" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I345" s="1"/>
     </row>
-    <row r="346" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I346" s="1"/>
     </row>
-    <row r="347" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I347" s="1"/>
     </row>
-    <row r="348" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I348" s="1"/>
     </row>
-    <row r="349" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I349" s="1"/>
     </row>
-    <row r="350" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I350" s="1"/>
     </row>
-    <row r="351" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I351" s="1"/>
     </row>
-    <row r="352" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I352" s="1"/>
     </row>
     <row r="353" spans="9:9" x14ac:dyDescent="0.25">

</xml_diff>